<commit_message>
Buat Import Nilai Asesmen
</commit_message>
<xml_diff>
--- a/src/SIAkademik/SIAkademik.Web/wwwroot/file/importTemplate/Template Import Data Tujuan Pembelajaran.xlsx
+++ b/src/SIAkademik/SIAkademik.Web/wwwroot/file/importTemplate/Template Import Data Tujuan Pembelajaran.xlsx
@@ -1230,7 +1230,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -1280,12 +1280,12 @@
       <c r="D5" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gQXPUUjSuG1RVATadoGOEKPq4ygqxwr2KC5fHeuQPLQe15cbFbqtkuvBPQsXq9tBrGbzjUTCdPKbfJokN+747A==" saltValue="Ws7RmvXpCoi4rVDCg30baQ==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" objects="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Vm+Gx2BlLeNA7pusO7slVNE327NnTSbSfco3mHYr8zTzBiE4Ea1aWavOAikGn/YHN11Y2idgjLXhJMbawbWPRA==" saltValue="p+JnN2d8G/GmWxiA0PdDWg==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" objects="1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5">
       <formula1>"E,F"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>